<commit_message>
feat: update Stage Task
调整关卡奖励 去掉首通奖励 增加通关任务奖励
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Task_任务.xlsx
+++ b/nevergiveup/Excel/Task_任务.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B4D6A0-6B71-46CE-953B-BBB7C01BBD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE302B21-75D1-40A1-950D-C47668970788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="278">
   <si>
     <t>int</t>
   </si>
@@ -271,9 +271,6 @@
     <t>通关世界1·困难</t>
   </si>
   <si>
-    <t>1|20||2|15||3|10</t>
-  </si>
-  <si>
     <t>Task_taskName_2</t>
   </si>
   <si>
@@ -922,16 +919,112 @@
     <t>今日解锁一个塔</t>
   </si>
   <si>
-    <t>1|50||2|40||3|15</t>
-  </si>
-  <si>
-    <t>1|50||2|30||3|10</t>
-  </si>
-  <si>
     <t>3|20</t>
   </si>
   <si>
-    <t>2|30||3|10</t>
+    <t>1|300||2|100||3|10</t>
+  </si>
+  <si>
+    <t>1|500||2|100||3|10</t>
+  </si>
+  <si>
+    <t>1|600||2|150||3|10</t>
+  </si>
+  <si>
+    <t>1|1000||2|200||3|10</t>
+  </si>
+  <si>
+    <t>1|2500||2|600||3|10</t>
+  </si>
+  <si>
+    <t>1|600||2|100||3|15</t>
+  </si>
+  <si>
+    <t>1|700||2|150||3|15</t>
+  </si>
+  <si>
+    <t>1|1000||2|200||3|15</t>
+  </si>
+  <si>
+    <t>1|1500||2|250||3|15</t>
+  </si>
+  <si>
+    <t>1|3500||2|900||3|15</t>
+  </si>
+  <si>
+    <t>1|100||2|100||3|10</t>
+  </si>
+  <si>
+    <t>1|300||2|200||3|10</t>
+  </si>
+  <si>
+    <t>1|300||2|300||3|10</t>
+  </si>
+  <si>
+    <t>1|2000||2|600||3|10</t>
+  </si>
+  <si>
+    <t>1|400||2|200||3|50</t>
+  </si>
+  <si>
+    <t>1|800||2|400||3|100</t>
+  </si>
+  <si>
+    <t>1|300||2|200||3|20</t>
+  </si>
+  <si>
+    <t>1|600||2|400||3|50</t>
+  </si>
+  <si>
+    <t>1|400||2|100||3|50</t>
+  </si>
+  <si>
+    <t>1|800||2|200||3|50</t>
+  </si>
+  <si>
+    <t>1|1000||2|300||3|50</t>
+  </si>
+  <si>
+    <t>1|2500||2|400||3|50</t>
+  </si>
+  <si>
+    <t>1|400||2|200||3|20</t>
+  </si>
+  <si>
+    <t>1|800||2|400||3|20</t>
+  </si>
+  <si>
+    <t>1|800||2|400</t>
+  </si>
+  <si>
+    <t>1|1000||2|600</t>
+  </si>
+  <si>
+    <t>1|1500||2|800</t>
+  </si>
+  <si>
+    <t>1|400||2|200</t>
+  </si>
+  <si>
+    <t>1|400||2|100||3|20</t>
+  </si>
+  <si>
+    <t>1|200||2|120||3|10</t>
+  </si>
+  <si>
+    <t>1|500||2|500||3|10</t>
+  </si>
+  <si>
+    <t>1|300||2|70||3|10</t>
+  </si>
+  <si>
+    <t>1|100||2|70||3|10</t>
+  </si>
+  <si>
+    <t>1|200||2|70||3|10</t>
+  </si>
+  <si>
+    <t>2|70||3|10</t>
   </si>
 </sst>
 </file>
@@ -1407,8 +1500,8 @@
   <dimension ref="A1:AMJ77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -1551,7 +1644,7 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="8" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -1565,20 +1658,20 @@
         <v>100002</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="E6" s="6">
         <v>1</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="8" t="s">
-        <v>26</v>
+        <v>244</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -1592,20 +1685,20 @@
         <v>100003</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="8" t="s">
-        <v>26</v>
+        <v>245</v>
       </c>
       <c r="H7" s="6">
         <v>1</v>
@@ -1619,20 +1712,20 @@
         <v>100004</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="E8" s="6">
         <v>1</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="8" t="s">
-        <v>26</v>
+        <v>246</v>
       </c>
       <c r="H8" s="6">
         <v>1</v>
@@ -1646,20 +1739,20 @@
         <v>100005</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="8" t="s">
-        <v>26</v>
+        <v>247</v>
       </c>
       <c r="H9" s="6">
         <v>1</v>
@@ -1673,20 +1766,20 @@
         <v>100006</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="8" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="H10" s="6">
         <v>7</v>
@@ -1700,20 +1793,20 @@
         <v>100007</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="E11" s="6">
         <v>1</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="8" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="H11" s="6">
         <v>7</v>
@@ -1727,20 +1820,20 @@
         <v>100008</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="E12" s="6">
         <v>1</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="8" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="H12" s="6">
         <v>7</v>
@@ -1754,20 +1847,20 @@
         <v>100009</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="E13" s="6">
         <v>1</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="8" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="H13" s="6">
         <v>7</v>
@@ -1781,20 +1874,20 @@
         <v>100010</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="8" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="H14" s="6">
         <v>7</v>
@@ -1808,20 +1901,20 @@
         <v>100011</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="E15" s="6">
         <v>1</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="8" t="s">
-        <v>26</v>
+        <v>253</v>
       </c>
       <c r="H15" s="6">
         <v>2</v>
@@ -1835,20 +1928,20 @@
         <v>100012</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="E16" s="6">
         <v>1</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="8" t="s">
-        <v>26</v>
+        <v>253</v>
       </c>
       <c r="H16" s="6">
         <v>2</v>
@@ -1862,20 +1955,20 @@
         <v>100013</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="8" t="s">
-        <v>26</v>
+        <v>253</v>
       </c>
       <c r="H17" s="6">
         <v>2</v>
@@ -1889,20 +1982,20 @@
         <v>100014</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="E18" s="6">
         <v>1</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="8" t="s">
-        <v>26</v>
+        <v>253</v>
       </c>
       <c r="H18" s="6">
         <v>2</v>
@@ -1916,20 +2009,20 @@
         <v>100015</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="E19" s="6">
         <v>1</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="8" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="H19" s="6">
         <v>1047</v>
@@ -1943,20 +2036,20 @@
         <v>100016</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="E20" s="6">
         <v>1</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="8" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="H20" s="6">
         <v>1048</v>
@@ -1970,20 +2063,20 @@
         <v>100017</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="E21" s="6">
         <v>1</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="8" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="H21" s="6">
         <v>1049</v>
@@ -1997,20 +2090,20 @@
         <v>100018</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>77</v>
       </c>
       <c r="E22" s="6">
         <v>1</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="8" t="s">
-        <v>26</v>
+        <v>243</v>
       </c>
       <c r="H22" s="6">
         <v>26</v>
@@ -2024,20 +2117,20 @@
         <v>100019</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="E23" s="6">
         <v>1</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="8" t="s">
-        <v>26</v>
+        <v>254</v>
       </c>
       <c r="H23" s="6">
         <v>26</v>
@@ -2051,20 +2144,20 @@
         <v>100020</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="E24" s="6">
         <v>1</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="8" t="s">
-        <v>26</v>
+        <v>255</v>
       </c>
       <c r="H24" s="6">
         <v>26</v>
@@ -2078,20 +2171,20 @@
         <v>100021</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="E25" s="6">
         <v>1</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="8" t="s">
-        <v>26</v>
+        <v>256</v>
       </c>
       <c r="H25" s="6">
         <v>3</v>
@@ -2105,20 +2198,20 @@
         <v>100022</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="8" t="s">
-        <v>26</v>
+        <v>257</v>
       </c>
       <c r="H26" s="6">
         <v>5</v>
@@ -2132,26 +2225,26 @@
         <v>100023</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="E27" s="6">
         <v>1</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="8" t="s">
-        <v>26</v>
+        <v>258</v>
       </c>
       <c r="H27" s="6">
         <v>5</v>
       </c>
       <c r="I27" s="6">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
@@ -2159,20 +2252,20 @@
         <v>100024</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="E28" s="6">
         <v>1</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="8" t="s">
-        <v>26</v>
+        <v>259</v>
       </c>
       <c r="H28" s="6">
         <v>8</v>
@@ -2186,20 +2279,20 @@
         <v>100025</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="E29" s="6">
         <v>1</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="8" t="s">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="H29" s="6">
         <v>8</v>
@@ -2213,26 +2306,26 @@
         <v>100026</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>101</v>
       </c>
       <c r="E30" s="6">
         <v>1</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="8" t="s">
-        <v>26</v>
+        <v>261</v>
       </c>
       <c r="H30" s="6">
         <v>6</v>
       </c>
       <c r="I30" s="6">
-        <v>1000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
@@ -2240,26 +2333,26 @@
         <v>100027</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>103</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="E31" s="6">
         <v>1</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="8" t="s">
-        <v>26</v>
+        <v>262</v>
       </c>
       <c r="H31" s="6">
         <v>6</v>
       </c>
       <c r="I31" s="6">
-        <v>2000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
@@ -2267,26 +2360,26 @@
         <v>100028</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="E32" s="6">
         <v>1</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="8" t="s">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="H32" s="6">
         <v>6</v>
       </c>
       <c r="I32" s="6">
-        <v>5000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
@@ -2294,26 +2387,26 @@
         <v>100029</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="E33" s="6">
         <v>1</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="8" t="s">
-        <v>26</v>
+        <v>264</v>
       </c>
       <c r="H33" s="6">
         <v>6</v>
       </c>
       <c r="I33" s="6">
-        <v>10000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
@@ -2321,26 +2414,26 @@
         <v>100030</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="E34" s="6">
         <v>1</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="8" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="H34" s="6">
         <v>9</v>
       </c>
       <c r="I34" s="6">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
@@ -2348,26 +2441,26 @@
         <v>100031</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>116</v>
       </c>
       <c r="E35" s="6">
         <v>1</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="8" t="s">
-        <v>26</v>
+        <v>266</v>
       </c>
       <c r="H35" s="6">
         <v>9</v>
       </c>
       <c r="I35" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
@@ -2375,26 +2468,26 @@
         <v>100032</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>119</v>
       </c>
       <c r="E36" s="6">
         <v>1</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="8" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="H36" s="6">
         <v>10</v>
       </c>
       <c r="I36" s="6">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
@@ -2402,26 +2495,26 @@
         <v>100033</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>122</v>
       </c>
       <c r="E37" s="6">
         <v>1</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="8" t="s">
-        <v>26</v>
+        <v>266</v>
       </c>
       <c r="H37" s="6">
         <v>10</v>
       </c>
       <c r="I37" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
@@ -2429,26 +2522,26 @@
         <v>100034</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>125</v>
       </c>
       <c r="E38" s="6">
         <v>1</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="8" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="H38" s="6">
         <v>11</v>
       </c>
       <c r="I38" s="6">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
@@ -2456,26 +2549,26 @@
         <v>100035</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>127</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>128</v>
       </c>
       <c r="E39" s="6">
         <v>1</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="8" t="s">
-        <v>26</v>
+        <v>266</v>
       </c>
       <c r="H39" s="6">
         <v>11</v>
       </c>
       <c r="I39" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
@@ -2483,26 +2576,26 @@
         <v>100036</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>131</v>
       </c>
       <c r="E40" s="6">
         <v>1</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="8" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="H40" s="6">
         <v>12</v>
       </c>
       <c r="I40" s="6">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
@@ -2510,26 +2603,26 @@
         <v>100037</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="D41" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>134</v>
       </c>
       <c r="E41" s="6">
         <v>1</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="8" t="s">
-        <v>26</v>
+        <v>266</v>
       </c>
       <c r="H41" s="6">
         <v>12</v>
       </c>
       <c r="I41" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
@@ -2537,26 +2630,26 @@
         <v>100038</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>137</v>
       </c>
       <c r="E42" s="6">
         <v>1</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="8" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="H42" s="6">
         <v>13</v>
       </c>
       <c r="I42" s="6">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
@@ -2564,26 +2657,26 @@
         <v>100039</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>139</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>140</v>
       </c>
       <c r="E43" s="6">
         <v>1</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="8" t="s">
-        <v>26</v>
+        <v>266</v>
       </c>
       <c r="H43" s="6">
         <v>13</v>
       </c>
       <c r="I43" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
@@ -2591,26 +2684,26 @@
         <v>100040</v>
       </c>
       <c r="B44" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="D44" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="E44" s="6">
         <v>1</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="8" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="H44" s="6">
         <v>14</v>
       </c>
       <c r="I44" s="6">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
@@ -2618,26 +2711,26 @@
         <v>100041</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="D45" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>146</v>
       </c>
       <c r="E45" s="6">
         <v>1</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="8" t="s">
-        <v>26</v>
+        <v>266</v>
       </c>
       <c r="H45" s="6">
         <v>14</v>
       </c>
       <c r="I45" s="6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
@@ -2645,20 +2738,20 @@
         <v>100042</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="D46" s="6" t="s">
         <v>148</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>149</v>
       </c>
       <c r="E46" s="6">
         <v>1</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="8" t="s">
-        <v>26</v>
+        <v>267</v>
       </c>
       <c r="H46" s="6">
         <v>15</v>
@@ -2672,20 +2765,20 @@
         <v>100043</v>
       </c>
       <c r="B47" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="E47" s="6">
         <v>1</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="8" t="s">
-        <v>26</v>
+        <v>268</v>
       </c>
       <c r="H47" s="6">
         <v>15</v>
@@ -2699,20 +2792,20 @@
         <v>100044</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="D48" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="E48" s="6">
         <v>1</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="8" t="s">
-        <v>26</v>
+        <v>269</v>
       </c>
       <c r="H48" s="6">
         <v>15</v>
@@ -2726,20 +2819,20 @@
         <v>100045</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="D49" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="E49" s="6">
         <v>1</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="8" t="s">
-        <v>26</v>
+        <v>270</v>
       </c>
       <c r="H49" s="6">
         <v>16</v>
@@ -2753,26 +2846,26 @@
         <v>100046</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="D50" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="E50" s="6">
         <v>1</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="8" t="s">
-        <v>26</v>
+        <v>270</v>
       </c>
       <c r="H50" s="6">
         <v>16</v>
       </c>
       <c r="I50" s="6">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.15">
@@ -2780,26 +2873,26 @@
         <v>100047</v>
       </c>
       <c r="B51" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="E51" s="6">
         <v>1</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="8" t="s">
-        <v>26</v>
+        <v>270</v>
       </c>
       <c r="H51" s="6">
         <v>16</v>
       </c>
       <c r="I51" s="6">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.15">
@@ -2807,26 +2900,26 @@
         <v>100048</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="D52" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="E52" s="6">
         <v>1</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="8" t="s">
-        <v>26</v>
+        <v>270</v>
       </c>
       <c r="H52" s="6">
         <v>16</v>
       </c>
       <c r="I52" s="6">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.15">
@@ -2834,20 +2927,20 @@
         <v>100049</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="D53" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="E53" s="6">
         <v>1</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="8" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="H53" s="6">
         <v>17</v>
@@ -2861,20 +2954,20 @@
         <v>100050</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="D54" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="E54" s="6">
         <v>1</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="8" t="s">
-        <v>26</v>
+        <v>266</v>
       </c>
       <c r="H54" s="6">
         <v>17</v>
@@ -2888,20 +2981,20 @@
         <v>100051</v>
       </c>
       <c r="B55" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="D55" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>176</v>
       </c>
       <c r="E55" s="6">
         <v>1</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="8" t="s">
-        <v>26</v>
+        <v>271</v>
       </c>
       <c r="H55" s="9">
         <v>18</v>
@@ -2915,20 +3008,20 @@
         <v>100052</v>
       </c>
       <c r="B56" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="D56" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="E56" s="6">
         <v>1</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="8" t="s">
-        <v>26</v>
+        <v>271</v>
       </c>
       <c r="H56" s="6">
         <v>19</v>
@@ -2942,20 +3035,20 @@
         <v>100053</v>
       </c>
       <c r="B57" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="D57" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>182</v>
       </c>
       <c r="E57" s="6">
         <v>1</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="8" t="s">
-        <v>26</v>
+        <v>271</v>
       </c>
       <c r="H57" s="6">
         <v>21</v>
@@ -2969,20 +3062,20 @@
         <v>100054</v>
       </c>
       <c r="B58" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="D58" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="E58" s="6">
         <v>1</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="8" t="s">
-        <v>26</v>
+        <v>271</v>
       </c>
       <c r="H58" s="6">
         <v>20</v>
@@ -2996,13 +3089,13 @@
         <v>100055</v>
       </c>
       <c r="B59" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="D59" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="E59" s="6">
         <v>2</v>
@@ -3011,7 +3104,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="H59" s="6">
         <v>5</v>
@@ -3025,13 +3118,13 @@
         <v>100056</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="D60" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="E60" s="6">
         <v>2</v>
@@ -3040,7 +3133,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>26</v>
+        <v>273</v>
       </c>
       <c r="H60" s="6">
         <v>8</v>
@@ -3054,13 +3147,13 @@
         <v>100057</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C61" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="D61" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="E61" s="6">
         <v>2</v>
@@ -3069,7 +3162,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>26</v>
+        <v>274</v>
       </c>
       <c r="H61" s="6">
         <v>22</v>
@@ -3083,13 +3176,13 @@
         <v>100058</v>
       </c>
       <c r="B62" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C62" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="D62" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="E62" s="6">
         <v>2</v>
@@ -3098,7 +3191,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>26</v>
+        <v>274</v>
       </c>
       <c r="H62" s="6">
         <v>6</v>
@@ -3112,13 +3205,13 @@
         <v>100059</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="D63" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="E63" s="6">
         <v>2</v>
@@ -3127,7 +3220,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>26</v>
+        <v>274</v>
       </c>
       <c r="H63" s="6">
         <v>23</v>
@@ -3141,13 +3234,13 @@
         <v>100060</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="D64" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="E64" s="6">
         <v>2</v>
@@ -3156,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H64" s="6">
         <v>9</v>
@@ -3170,13 +3263,13 @@
         <v>100061</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C65" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="D65" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="E65" s="6">
         <v>2</v>
@@ -3185,7 +3278,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H65" s="6">
         <v>10</v>
@@ -3199,13 +3292,13 @@
         <v>100062</v>
       </c>
       <c r="B66" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C66" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="D66" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>209</v>
       </c>
       <c r="E66" s="6">
         <v>2</v>
@@ -3214,7 +3307,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H66" s="6">
         <v>11</v>
@@ -3228,13 +3321,13 @@
         <v>100063</v>
       </c>
       <c r="B67" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C67" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="D67" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="E67" s="6">
         <v>2</v>
@@ -3243,7 +3336,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H67" s="6">
         <v>12</v>
@@ -3257,13 +3350,13 @@
         <v>100064</v>
       </c>
       <c r="B68" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C68" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="D68" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="E68" s="6">
         <v>2</v>
@@ -3272,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H68" s="6">
         <v>13</v>
@@ -3286,13 +3379,13 @@
         <v>100065</v>
       </c>
       <c r="B69" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="D69" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="E69" s="6">
         <v>2</v>
@@ -3301,7 +3394,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H69" s="6">
         <v>14</v>
@@ -3315,13 +3408,13 @@
         <v>100066</v>
       </c>
       <c r="B70" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="D70" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="E70" s="6">
         <v>2</v>
@@ -3330,7 +3423,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H70" s="6">
         <v>17</v>
@@ -3344,13 +3437,13 @@
         <v>100067</v>
       </c>
       <c r="B71" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="D71" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="E71" s="6">
         <v>2</v>
@@ -3359,7 +3452,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H71" s="6">
         <v>18</v>
@@ -3373,13 +3466,13 @@
         <v>100068</v>
       </c>
       <c r="B72" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C72" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="D72" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>227</v>
       </c>
       <c r="E72" s="6">
         <v>2</v>
@@ -3388,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H72" s="6">
         <v>19</v>
@@ -3402,13 +3495,13 @@
         <v>100069</v>
       </c>
       <c r="B73" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C73" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="D73" s="6" t="s">
         <v>229</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>230</v>
       </c>
       <c r="E73" s="6">
         <v>2</v>
@@ -3417,7 +3510,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H73" s="6">
         <v>21</v>
@@ -3431,13 +3524,13 @@
         <v>100070</v>
       </c>
       <c r="B74" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C74" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="D74" s="6" t="s">
         <v>232</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>233</v>
       </c>
       <c r="E74" s="6">
         <v>2</v>
@@ -3446,7 +3539,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>26</v>
+        <v>275</v>
       </c>
       <c r="H74" s="6">
         <v>20</v>
@@ -3460,13 +3553,13 @@
         <v>100071</v>
       </c>
       <c r="B75" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C75" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="D75" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>236</v>
       </c>
       <c r="E75" s="6">
         <v>2</v>
@@ -3475,7 +3568,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
       <c r="H75" s="6">
         <v>15</v>
@@ -3489,13 +3582,13 @@
         <v>100072</v>
       </c>
       <c r="B76" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C76" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="D76" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>239</v>
       </c>
       <c r="E76" s="6">
         <v>2</v>
@@ -3504,7 +3597,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H76" s="6">
         <v>2</v>
@@ -3518,13 +3611,13 @@
         <v>100073</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C77" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="D77" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="E77" s="6">
         <v>2</v>
@@ -3533,7 +3626,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>246</v>
+        <v>277</v>
       </c>
       <c r="H77" s="6">
         <v>25</v>

</xml_diff>

<commit_message>
feat: add level up count
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Task_任务.xlsx
+++ b/nevergiveup/Excel/Task_任务.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF85AD56-2D3A-46A0-945F-BB6BF9A22A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -95,12 +91,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">任务类型
 </t>
     </r>
@@ -108,7 +98,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>1.</t>
     </r>
@@ -116,7 +106,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>通过某关卡</t>
@@ -125,7 +114,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>id
 2.</t>
@@ -134,7 +123,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>解锁科技树某</t>
@@ -143,7 +131,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>id</t>
     </r>
@@ -151,7 +139,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">科技
@@ -161,7 +148,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>3.</t>
     </r>
@@ -169,7 +156,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">解锁多少个塔
@@ -179,7 +165,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>4.</t>
     </r>
@@ -187,7 +173,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">副本获得多少星星
@@ -197,7 +182,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>5.</t>
     </r>
@@ -205,7 +190,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t xml:space="preserve">游玩几局游戏
@@ -215,7 +199,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>6.</t>
     </r>
@@ -223,7 +207,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="微软雅黑"/>
-        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>击败多少只怪物
@@ -247,6 +230,7 @@
 24.升级防御塔的次数
 25.日常解锁一次塔（只支持日常）
 26.累计天赋解锁
+27.人物升级的等级数
 1047.终极天赋物理
 1048.终极天赋魔法
 1049.终极天赋耐久</t>
@@ -271,6 +255,9 @@
     <t>通关世界1·困难</t>
   </si>
   <si>
+    <t>1|300||2|100||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_2</t>
   </si>
   <si>
@@ -280,6 +267,9 @@
     <t>通关世界2·困难</t>
   </si>
   <si>
+    <t>1|500||2|100||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_3</t>
   </si>
   <si>
@@ -289,6 +279,9 @@
     <t>通关世界3·困难</t>
   </si>
   <si>
+    <t>1|600||2|150||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_4</t>
   </si>
   <si>
@@ -298,6 +291,9 @@
     <t>通关世界4·困难</t>
   </si>
   <si>
+    <t>1|1000||2|200||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_5</t>
   </si>
   <si>
@@ -307,6 +303,9 @@
     <t>通关世界5·困难</t>
   </si>
   <si>
+    <t>1|2500||2|600||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_6</t>
   </si>
   <si>
@@ -316,6 +315,9 @@
     <t>完美通关世界1·困难</t>
   </si>
   <si>
+    <t>1|600||2|100||3|15</t>
+  </si>
+  <si>
     <t>Task_taskName_7</t>
   </si>
   <si>
@@ -325,6 +327,9 @@
     <t>完美通关世界2·困难</t>
   </si>
   <si>
+    <t>1|700||2|150||3|15</t>
+  </si>
+  <si>
     <t>Task_taskName_8</t>
   </si>
   <si>
@@ -334,6 +339,9 @@
     <t>完美通关世界3·困难</t>
   </si>
   <si>
+    <t>1|1000||2|200||3|15</t>
+  </si>
+  <si>
     <t>Task_taskName_9</t>
   </si>
   <si>
@@ -343,6 +351,9 @@
     <t>完美通关世界4·困难</t>
   </si>
   <si>
+    <t>1|1500||2|250||3|15</t>
+  </si>
+  <si>
     <t>Task_taskName_10</t>
   </si>
   <si>
@@ -352,6 +363,9 @@
     <t>完美通关世界5·困难</t>
   </si>
   <si>
+    <t>1|3500||2|900||3|15</t>
+  </si>
+  <si>
     <t>Task_taskName_11</t>
   </si>
   <si>
@@ -361,6 +375,9 @@
     <t>解锁天赋·慧光</t>
   </si>
   <si>
+    <t>1|100||2|100||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_12</t>
   </si>
   <si>
@@ -433,6 +450,9 @@
     <t>累计解锁天赋120点</t>
   </si>
   <si>
+    <t>1|400||2|200||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_20</t>
   </si>
   <si>
@@ -442,6 +462,9 @@
     <t>累计解锁天赋150点</t>
   </si>
   <si>
+    <t>1|500||2|300||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_21</t>
   </si>
   <si>
@@ -451,6 +474,9 @@
     <t>解锁塔38个</t>
   </si>
   <si>
+    <t>1|2000||2|600||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_22</t>
   </si>
   <si>
@@ -460,6 +486,9 @@
     <t>累计游戏100次</t>
   </si>
   <si>
+    <t>1|400||2|200||3|50</t>
+  </si>
+  <si>
     <t>Task_taskName_23</t>
   </si>
   <si>
@@ -469,6 +498,9 @@
     <t>累计游戏200次</t>
   </si>
   <si>
+    <t>1|800||2|400||3|100</t>
+  </si>
+  <si>
     <t>Task_taskName_24</t>
   </si>
   <si>
@@ -478,6 +510,9 @@
     <t>累计完美通关20次</t>
   </si>
   <si>
+    <t>1|300||2|200||3|20</t>
+  </si>
+  <si>
     <t>Task_taskName_25</t>
   </si>
   <si>
@@ -487,6 +522,9 @@
     <t>累计完美通关50次</t>
   </si>
   <si>
+    <t>1|600||2|400||3|50</t>
+  </si>
+  <si>
     <t>Task_taskName_26</t>
   </si>
   <si>
@@ -496,6 +534,9 @@
     <t>累计击败怪物1000个</t>
   </si>
   <si>
+    <t>1|400||2|100||3|50</t>
+  </si>
+  <si>
     <t>Task_taskName_27</t>
   </si>
   <si>
@@ -505,6 +546,9 @@
     <t>累计击败怪物2000个</t>
   </si>
   <si>
+    <t>1|800||2|200||3|50</t>
+  </si>
+  <si>
     <t>Task_taskName_28</t>
   </si>
   <si>
@@ -514,6 +558,9 @@
     <t>累计击败怪物5000个</t>
   </si>
   <si>
+    <t>1|1000||2|300||3|50</t>
+  </si>
+  <si>
     <t>Task_taskName_29</t>
   </si>
   <si>
@@ -523,6 +570,9 @@
     <t>累计击败怪物10000个</t>
   </si>
   <si>
+    <t>1|2500||2|400||3|50</t>
+  </si>
+  <si>
     <t>Task_taskName_30</t>
   </si>
   <si>
@@ -532,6 +582,9 @@
     <t>累计部署光元素塔500次</t>
   </si>
   <si>
+    <t>1|400||2|200||3|20</t>
+  </si>
+  <si>
     <t>Task_taskName_31</t>
   </si>
   <si>
@@ -541,6 +594,9 @@
     <t>累计部署光元素塔1000次</t>
   </si>
   <si>
+    <t>1|800||2|400||3|20</t>
+  </si>
+  <si>
     <t>Task_taskName_32</t>
   </si>
   <si>
@@ -640,6 +696,9 @@
     <t>角色等级到达18级</t>
   </si>
   <si>
+    <t>1|800||2|400</t>
+  </si>
+  <si>
     <t>Task_taskName_43</t>
   </si>
   <si>
@@ -649,6 +708,9 @@
     <t>角色等级到达30级</t>
   </si>
   <si>
+    <t>1|1000||2|600</t>
+  </si>
+  <si>
     <t>Task_taskName_44</t>
   </si>
   <si>
@@ -658,6 +720,9 @@
     <t>角色等级到达50级</t>
   </si>
   <si>
+    <t>1|1500||2|800</t>
+  </si>
+  <si>
     <t>Task_taskName_45</t>
   </si>
   <si>
@@ -667,6 +732,9 @@
     <t>无尽关卡成功抵御10波</t>
   </si>
   <si>
+    <t>1|400||2|200</t>
+  </si>
+  <si>
     <t>Task_taskName_46</t>
   </si>
   <si>
@@ -676,6 +744,9 @@
     <t>无尽关卡成功抵御30波</t>
   </si>
   <si>
+    <t>1|600||2|300</t>
+  </si>
+  <si>
     <t>Task_taskName_47</t>
   </si>
   <si>
@@ -694,6 +765,9 @@
     <t>无尽关卡成功抵御100波</t>
   </si>
   <si>
+    <t>1|1000||2|500</t>
+  </si>
+  <si>
     <t>Task_taskName_49</t>
   </si>
   <si>
@@ -712,6 +786,9 @@
     <t>累计强化3级塔1000次</t>
   </si>
   <si>
+    <t>1|1200||2|600||3|60</t>
+  </si>
+  <si>
     <t>Task_taskName_51</t>
   </si>
   <si>
@@ -721,6 +798,9 @@
     <t>累计击败复原力怪物2000只</t>
   </si>
   <si>
+    <t>1|400||2|100||3|20</t>
+  </si>
+  <si>
     <t>Task_taskName_52</t>
   </si>
   <si>
@@ -757,6 +837,9 @@
     <t>今日游戏10次</t>
   </si>
   <si>
+    <t>1|200||2|120||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_56</t>
   </si>
   <si>
@@ -766,6 +849,9 @@
     <t>今日完美通关10次</t>
   </si>
   <si>
+    <t>1|500||2|500||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_57</t>
   </si>
   <si>
@@ -775,6 +861,9 @@
     <t>今日挑战无尽关卡3次</t>
   </si>
   <si>
+    <t>1|300||2|70||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_58</t>
   </si>
   <si>
@@ -802,6 +891,9 @@
     <t>今日部署光元素塔200次</t>
   </si>
   <si>
+    <t>1|100||2|70||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_61</t>
   </si>
   <si>
@@ -901,6 +993,9 @@
     <t>今日角色完成一次升级</t>
   </si>
   <si>
+    <t>1|200||2|70||3|10</t>
+  </si>
+  <si>
     <t>Task_taskName_72</t>
   </si>
   <si>
@@ -910,6 +1005,9 @@
     <t>今日解锁一点天赋</t>
   </si>
   <si>
+    <t>3|20</t>
+  </si>
+  <si>
     <t>Task_taskName_73</t>
   </si>
   <si>
@@ -919,128 +1017,20 @@
     <t>今日解锁一个塔</t>
   </si>
   <si>
-    <t>3|20</t>
-  </si>
-  <si>
-    <t>1|300||2|100||3|10</t>
-  </si>
-  <si>
-    <t>1|500||2|100||3|10</t>
-  </si>
-  <si>
-    <t>1|600||2|150||3|10</t>
-  </si>
-  <si>
-    <t>1|1000||2|200||3|10</t>
-  </si>
-  <si>
-    <t>1|2500||2|600||3|10</t>
-  </si>
-  <si>
-    <t>1|600||2|100||3|15</t>
-  </si>
-  <si>
-    <t>1|700||2|150||3|15</t>
-  </si>
-  <si>
-    <t>1|1000||2|200||3|15</t>
-  </si>
-  <si>
-    <t>1|1500||2|250||3|15</t>
-  </si>
-  <si>
-    <t>1|3500||2|900||3|15</t>
-  </si>
-  <si>
-    <t>1|100||2|100||3|10</t>
-  </si>
-  <si>
-    <t>1|2000||2|600||3|10</t>
-  </si>
-  <si>
-    <t>1|400||2|200||3|50</t>
-  </si>
-  <si>
-    <t>1|800||2|400||3|100</t>
-  </si>
-  <si>
-    <t>1|300||2|200||3|20</t>
-  </si>
-  <si>
-    <t>1|600||2|400||3|50</t>
-  </si>
-  <si>
-    <t>1|400||2|100||3|50</t>
-  </si>
-  <si>
-    <t>1|800||2|200||3|50</t>
-  </si>
-  <si>
-    <t>1|1000||2|300||3|50</t>
-  </si>
-  <si>
-    <t>1|2500||2|400||3|50</t>
-  </si>
-  <si>
-    <t>1|400||2|200||3|20</t>
-  </si>
-  <si>
-    <t>1|800||2|400||3|20</t>
-  </si>
-  <si>
-    <t>1|800||2|400</t>
-  </si>
-  <si>
-    <t>1|1000||2|600</t>
-  </si>
-  <si>
-    <t>1|1500||2|800</t>
-  </si>
-  <si>
-    <t>1|400||2|200</t>
-  </si>
-  <si>
-    <t>1|400||2|100||3|20</t>
-  </si>
-  <si>
-    <t>1|200||2|120||3|10</t>
-  </si>
-  <si>
-    <t>1|500||2|500||3|10</t>
-  </si>
-  <si>
-    <t>1|300||2|70||3|10</t>
-  </si>
-  <si>
-    <t>1|100||2|70||3|10</t>
-  </si>
-  <si>
-    <t>1|200||2|70||3|10</t>
-  </si>
-  <si>
     <t>2|70||3|10</t>
-  </si>
-  <si>
-    <t>1|400||2|200||3|10</t>
-  </si>
-  <si>
-    <t>1|500||2|300||3|10</t>
-  </si>
-  <si>
-    <t>1|600||2|300</t>
-  </si>
-  <si>
-    <t>1|1000||2|500</t>
-  </si>
-  <si>
-    <t>1|1200||2|600||3|60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1051,13 +1041,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1065,28 +1053,172 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1101,12 +1233,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1129,13 +1441,255 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1163,162 +1717,90 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
       <border>
@@ -1329,7 +1811,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -1357,40 +1839,154 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
+          <color theme="4" tint="0.399975585192419"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
-      <tableStyleElement type="pageFieldValues" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1449,7 +2045,7 @@
         <a:cs typeface="DejaVu Sans"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1500,35 +2096,36 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="27.375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="26.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="42.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.125" customWidth="1"/>
-    <col min="8" max="9" width="25.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.3727272727273" style="2" customWidth="1"/>
+    <col min="3" max="5" width="26.1272727272727" style="2" customWidth="1"/>
+    <col min="6" max="6" width="42.6272727272727" style="2" customWidth="1"/>
+    <col min="7" max="7" width="18.1272727272727" customWidth="1"/>
+    <col min="8" max="9" width="25.2545454545455" style="2" customWidth="1"/>
     <col min="10" max="978" width="9" style="2"/>
-    <col min="979" max="985" width="11.625" style="2" customWidth="1"/>
+    <col min="979" max="985" width="11.6272727272727" style="2" customWidth="1"/>
     <col min="986" max="986" width="9" style="2"/>
-    <col min="987" max="997" width="11.625" style="2" customWidth="1"/>
+    <col min="987" max="997" width="11.6272727272727" style="2" customWidth="1"/>
     <col min="998" max="1024" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +2155,7 @@
       </c>
       <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" s="1" customFormat="1" ht="14.5" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1588,7 +2185,7 @@
       </c>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" s="1" customFormat="1" ht="408" customHeight="1" spans="1:10">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1618,7 +2215,7 @@
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" s="1" customFormat="1" ht="14.5" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1635,7 +2232,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9">
       <c r="A5" s="6">
         <v>100001</v>
       </c>
@@ -1653,7 +2250,7 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="8" t="s">
-        <v>243</v>
+        <v>26</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -1662,25 +2259,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9">
       <c r="A6" s="6">
         <v>100002</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="6">
         <v>1</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="8" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="H6" s="6">
         <v>1</v>
@@ -1689,25 +2286,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9">
       <c r="A7" s="6">
         <v>100003</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E7" s="6">
         <v>1</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="8" t="s">
-        <v>245</v>
+        <v>34</v>
       </c>
       <c r="H7" s="6">
         <v>1</v>
@@ -1716,25 +2313,25 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9">
       <c r="A8" s="6">
         <v>100004</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E8" s="6">
         <v>1</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="8" t="s">
-        <v>246</v>
+        <v>38</v>
       </c>
       <c r="H8" s="6">
         <v>1</v>
@@ -1743,25 +2340,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9">
       <c r="A9" s="6">
         <v>100005</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E9" s="6">
         <v>1</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="8" t="s">
-        <v>247</v>
+        <v>42</v>
       </c>
       <c r="H9" s="6">
         <v>1</v>
@@ -1770,25 +2367,25 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9">
       <c r="A10" s="6">
         <v>100006</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E10" s="6">
         <v>1</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="8" t="s">
-        <v>248</v>
+        <v>46</v>
       </c>
       <c r="H10" s="6">
         <v>7</v>
@@ -1797,25 +2394,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9">
       <c r="A11" s="6">
         <v>100007</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E11" s="6">
         <v>1</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="8" t="s">
-        <v>249</v>
+        <v>50</v>
       </c>
       <c r="H11" s="6">
         <v>7</v>
@@ -1824,25 +2421,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9">
       <c r="A12" s="6">
         <v>100008</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E12" s="6">
         <v>1</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="8" t="s">
-        <v>250</v>
+        <v>54</v>
       </c>
       <c r="H12" s="6">
         <v>7</v>
@@ -1851,25 +2448,25 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9">
       <c r="A13" s="6">
         <v>100009</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E13" s="6">
         <v>1</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="8" t="s">
-        <v>251</v>
+        <v>58</v>
       </c>
       <c r="H13" s="6">
         <v>7</v>
@@ -1878,25 +2475,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9">
       <c r="A14" s="6">
         <v>100010</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E14" s="6">
         <v>1</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="8" t="s">
-        <v>252</v>
+        <v>62</v>
       </c>
       <c r="H14" s="6">
         <v>7</v>
@@ -1905,25 +2502,25 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:9">
       <c r="A15" s="6">
         <v>100011</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E15" s="6">
         <v>1</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="8" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="H15" s="6">
         <v>2</v>
@@ -1932,25 +2529,25 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9">
       <c r="A16" s="6">
         <v>100012</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E16" s="6">
         <v>1</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="8" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="H16" s="6">
         <v>2</v>
@@ -1959,25 +2556,25 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:9">
       <c r="A17" s="6">
         <v>100013</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E17" s="6">
         <v>1</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="8" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="H17" s="6">
         <v>2</v>
@@ -1986,25 +2583,25 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9">
       <c r="A18" s="6">
         <v>100014</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="E18" s="6">
         <v>1</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="8" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="H18" s="6">
         <v>2</v>
@@ -2013,25 +2610,25 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9">
       <c r="A19" s="6">
         <v>100015</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E19" s="6">
         <v>1</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="8" t="s">
-        <v>243</v>
+        <v>26</v>
       </c>
       <c r="H19" s="6">
         <v>1047</v>
@@ -2040,25 +2637,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:9">
       <c r="A20" s="6">
         <v>100016</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="E20" s="6">
         <v>1</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="8" t="s">
-        <v>243</v>
+        <v>26</v>
       </c>
       <c r="H20" s="6">
         <v>1048</v>
@@ -2067,25 +2664,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9">
       <c r="A21" s="6">
         <v>100017</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E21" s="6">
         <v>1</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="8" t="s">
-        <v>243</v>
+        <v>26</v>
       </c>
       <c r="H21" s="6">
         <v>1049</v>
@@ -2094,25 +2691,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:9">
       <c r="A22" s="6">
         <v>100018</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E22" s="6">
         <v>1</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="8" t="s">
-        <v>243</v>
+        <v>26</v>
       </c>
       <c r="H22" s="6">
         <v>26</v>
@@ -2121,25 +2718,25 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:9">
       <c r="A23" s="6">
         <v>100019</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="E23" s="6">
         <v>1</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="8" t="s">
-        <v>276</v>
+        <v>91</v>
       </c>
       <c r="H23" s="6">
         <v>26</v>
@@ -2148,25 +2745,25 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9">
       <c r="A24" s="6">
         <v>100020</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E24" s="6">
         <v>1</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="8" t="s">
-        <v>277</v>
+        <v>95</v>
       </c>
       <c r="H24" s="6">
         <v>26</v>
@@ -2175,25 +2772,25 @@
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9">
       <c r="A25" s="6">
         <v>100021</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="E25" s="6">
         <v>1</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="8" t="s">
-        <v>254</v>
+        <v>99</v>
       </c>
       <c r="H25" s="6">
         <v>3</v>
@@ -2202,25 +2799,25 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9">
       <c r="A26" s="6">
         <v>100022</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="E26" s="6">
         <v>1</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="8" t="s">
-        <v>255</v>
+        <v>103</v>
       </c>
       <c r="H26" s="6">
         <v>5</v>
@@ -2229,25 +2826,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9">
       <c r="A27" s="6">
         <v>100023</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E27" s="6">
         <v>1</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="8" t="s">
-        <v>256</v>
+        <v>107</v>
       </c>
       <c r="H27" s="6">
         <v>5</v>
@@ -2256,25 +2853,25 @@
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9">
       <c r="A28" s="6">
         <v>100024</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="E28" s="6">
         <v>1</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="8" t="s">
-        <v>257</v>
+        <v>111</v>
       </c>
       <c r="H28" s="6">
         <v>8</v>
@@ -2283,25 +2880,25 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9">
       <c r="A29" s="6">
         <v>100025</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="E29" s="6">
         <v>1</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="8" t="s">
-        <v>258</v>
+        <v>115</v>
       </c>
       <c r="H29" s="6">
         <v>8</v>
@@ -2310,25 +2907,25 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:9">
       <c r="A30" s="6">
         <v>100026</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="E30" s="6">
         <v>1</v>
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="8" t="s">
-        <v>259</v>
+        <v>119</v>
       </c>
       <c r="H30" s="6">
         <v>6</v>
@@ -2337,25 +2934,25 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9">
       <c r="A31" s="6">
         <v>100027</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="E31" s="6">
         <v>1</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="8" t="s">
-        <v>260</v>
+        <v>123</v>
       </c>
       <c r="H31" s="6">
         <v>6</v>
@@ -2364,25 +2961,25 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9">
       <c r="A32" s="6">
         <v>100028</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="E32" s="6">
         <v>1</v>
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="8" t="s">
-        <v>261</v>
+        <v>127</v>
       </c>
       <c r="H32" s="6">
         <v>6</v>
@@ -2391,25 +2988,25 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9">
       <c r="A33" s="6">
         <v>100029</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="E33" s="6">
         <v>1</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="8" t="s">
-        <v>262</v>
+        <v>131</v>
       </c>
       <c r="H33" s="6">
         <v>6</v>
@@ -2418,25 +3015,25 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9">
       <c r="A34" s="6">
         <v>100030</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="E34" s="6">
         <v>1</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="8" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="H34" s="6">
         <v>9</v>
@@ -2445,25 +3042,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:9">
       <c r="A35" s="6">
         <v>100031</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="E35" s="6">
         <v>1</v>
       </c>
       <c r="F35" s="6"/>
       <c r="G35" s="8" t="s">
-        <v>264</v>
+        <v>139</v>
       </c>
       <c r="H35" s="6">
         <v>9</v>
@@ -2472,25 +3069,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:9">
       <c r="A36" s="6">
         <v>100032</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="E36" s="6">
         <v>1</v>
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="8" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="H36" s="6">
         <v>10</v>
@@ -2499,25 +3096,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:9">
       <c r="A37" s="6">
         <v>100033</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="E37" s="6">
         <v>1</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="8" t="s">
-        <v>264</v>
+        <v>139</v>
       </c>
       <c r="H37" s="6">
         <v>10</v>
@@ -2526,25 +3123,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9">
       <c r="A38" s="6">
         <v>100034</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="E38" s="6">
         <v>1</v>
       </c>
       <c r="F38" s="6"/>
       <c r="G38" s="8" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="H38" s="6">
         <v>11</v>
@@ -2553,25 +3150,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9">
       <c r="A39" s="6">
         <v>100035</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="E39" s="6">
         <v>1</v>
       </c>
       <c r="F39" s="6"/>
       <c r="G39" s="8" t="s">
-        <v>264</v>
+        <v>139</v>
       </c>
       <c r="H39" s="6">
         <v>11</v>
@@ -2580,25 +3177,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9">
       <c r="A40" s="6">
         <v>100036</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="E40" s="6">
         <v>1</v>
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="8" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="H40" s="6">
         <v>12</v>
@@ -2607,25 +3204,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9">
       <c r="A41" s="6">
         <v>100037</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="E41" s="6">
         <v>1</v>
       </c>
       <c r="F41" s="6"/>
       <c r="G41" s="8" t="s">
-        <v>264</v>
+        <v>139</v>
       </c>
       <c r="H41" s="6">
         <v>12</v>
@@ -2634,25 +3231,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9">
       <c r="A42" s="6">
         <v>100038</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="E42" s="6">
         <v>1</v>
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="8" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="H42" s="6">
         <v>13</v>
@@ -2661,25 +3258,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9">
       <c r="A43" s="6">
         <v>100039</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="E43" s="6">
         <v>1</v>
       </c>
       <c r="F43" s="6"/>
       <c r="G43" s="8" t="s">
-        <v>264</v>
+        <v>139</v>
       </c>
       <c r="H43" s="6">
         <v>13</v>
@@ -2688,25 +3285,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9">
       <c r="A44" s="6">
         <v>100040</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="E44" s="6">
         <v>1</v>
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="8" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="H44" s="6">
         <v>14</v>
@@ -2715,25 +3312,25 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9">
       <c r="A45" s="6">
         <v>100041</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="E45" s="6">
         <v>1</v>
       </c>
       <c r="F45" s="6"/>
       <c r="G45" s="8" t="s">
-        <v>264</v>
+        <v>139</v>
       </c>
       <c r="H45" s="6">
         <v>14</v>
@@ -2742,25 +3339,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9">
       <c r="A46" s="6">
         <v>100042</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="E46" s="6">
         <v>1</v>
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="8" t="s">
-        <v>265</v>
+        <v>173</v>
       </c>
       <c r="H46" s="6">
         <v>15</v>
@@ -2769,25 +3366,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9">
       <c r="A47" s="6">
         <v>100043</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="E47" s="6">
         <v>1</v>
       </c>
       <c r="F47" s="6"/>
       <c r="G47" s="8" t="s">
-        <v>266</v>
+        <v>177</v>
       </c>
       <c r="H47" s="6">
         <v>15</v>
@@ -2796,25 +3393,25 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9">
       <c r="A48" s="6">
         <v>100044</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="E48" s="6">
         <v>1</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="8" t="s">
-        <v>267</v>
+        <v>181</v>
       </c>
       <c r="H48" s="6">
         <v>15</v>
@@ -2823,25 +3420,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:9">
       <c r="A49" s="6">
         <v>100045</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>156</v>
+        <v>183</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>157</v>
+        <v>184</v>
       </c>
       <c r="E49" s="6">
         <v>1</v>
       </c>
       <c r="F49" s="6"/>
       <c r="G49" s="8" t="s">
-        <v>268</v>
+        <v>185</v>
       </c>
       <c r="H49" s="6">
         <v>16</v>
@@ -2850,25 +3447,25 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9">
       <c r="A50" s="6">
         <v>100046</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="E50" s="6">
         <v>1</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="8" t="s">
-        <v>278</v>
+        <v>189</v>
       </c>
       <c r="H50" s="6">
         <v>16</v>
@@ -2877,25 +3474,25 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:9">
       <c r="A51" s="6">
         <v>100047</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>162</v>
+        <v>191</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="E51" s="6">
         <v>1</v>
       </c>
       <c r="F51" s="6"/>
       <c r="G51" s="8" t="s">
-        <v>265</v>
+        <v>173</v>
       </c>
       <c r="H51" s="6">
         <v>16</v>
@@ -2904,25 +3501,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9">
       <c r="A52" s="6">
         <v>100048</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="E52" s="6">
         <v>1</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="8" t="s">
-        <v>279</v>
+        <v>196</v>
       </c>
       <c r="H52" s="6">
         <v>16</v>
@@ -2931,25 +3528,25 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9">
       <c r="A53" s="6">
         <v>100049</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="E53" s="6">
         <v>1</v>
       </c>
       <c r="F53" s="6"/>
       <c r="G53" s="8" t="s">
-        <v>263</v>
+        <v>135</v>
       </c>
       <c r="H53" s="6">
         <v>17</v>
@@ -2958,79 +3555,79 @@
         <v>500</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9">
       <c r="A54" s="6">
         <v>100050</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="E54" s="6">
         <v>1</v>
       </c>
-      <c r="F54" s="9"/>
+      <c r="F54" s="6"/>
       <c r="G54" s="8" t="s">
-        <v>280</v>
+        <v>203</v>
       </c>
       <c r="H54" s="6">
         <v>17</v>
       </c>
-      <c r="I54" s="9">
+      <c r="I54" s="6">
         <v>2000</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9">
       <c r="A55" s="6">
         <v>100051</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>175</v>
+        <v>205</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>206</v>
       </c>
       <c r="E55" s="6">
         <v>1</v>
       </c>
-      <c r="F55" s="9"/>
+      <c r="F55" s="6"/>
       <c r="G55" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="H55" s="9">
+        <v>207</v>
+      </c>
+      <c r="H55" s="6">
         <v>18</v>
       </c>
-      <c r="I55" s="9">
+      <c r="I55" s="6">
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9">
       <c r="A56" s="6">
         <v>100052</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="E56" s="6">
         <v>1</v>
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="8" t="s">
-        <v>269</v>
+        <v>207</v>
       </c>
       <c r="H56" s="6">
         <v>19</v>
@@ -3039,25 +3636,25 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:9">
       <c r="A57" s="6">
         <v>100053</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>179</v>
+        <v>211</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>181</v>
+        <v>212</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="E57" s="6">
         <v>1</v>
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="8" t="s">
-        <v>269</v>
+        <v>207</v>
       </c>
       <c r="H57" s="6">
         <v>21</v>
@@ -3066,25 +3663,25 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9">
       <c r="A58" s="6">
         <v>100054</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="E58" s="6">
         <v>1</v>
       </c>
-      <c r="F58" s="9"/>
+      <c r="F58" s="6"/>
       <c r="G58" s="8" t="s">
-        <v>269</v>
+        <v>207</v>
       </c>
       <c r="H58" s="6">
         <v>20</v>
@@ -3093,18 +3690,18 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:9">
       <c r="A59" s="6">
         <v>100055</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>185</v>
+        <v>217</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="E59" s="6">
         <v>2</v>
@@ -3113,7 +3710,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="H59" s="6">
         <v>5</v>
@@ -3122,18 +3719,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9">
       <c r="A60" s="6">
         <v>100056</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>189</v>
+        <v>222</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>190</v>
+        <v>223</v>
       </c>
       <c r="E60" s="6">
         <v>2</v>
@@ -3142,7 +3739,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>271</v>
+        <v>224</v>
       </c>
       <c r="H60" s="6">
         <v>8</v>
@@ -3151,18 +3748,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:9">
       <c r="A61" s="6">
         <v>100057</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>191</v>
+        <v>225</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="E61" s="6">
         <v>2</v>
@@ -3171,7 +3768,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>272</v>
+        <v>228</v>
       </c>
       <c r="H61" s="6">
         <v>22</v>
@@ -3180,18 +3777,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9">
       <c r="A62" s="6">
         <v>100058</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>194</v>
+        <v>229</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>196</v>
+        <v>231</v>
       </c>
       <c r="E62" s="6">
         <v>2</v>
@@ -3200,7 +3797,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>272</v>
+        <v>228</v>
       </c>
       <c r="H62" s="6">
         <v>6</v>
@@ -3209,18 +3806,18 @@
         <v>300</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:9">
       <c r="A63" s="6">
         <v>100059</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>197</v>
+        <v>232</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="E63" s="6">
         <v>2</v>
@@ -3229,7 +3826,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>272</v>
+        <v>228</v>
       </c>
       <c r="H63" s="6">
         <v>23</v>
@@ -3238,18 +3835,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9">
       <c r="A64" s="6">
         <v>100060</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>200</v>
+        <v>235</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="E64" s="6">
         <v>2</v>
@@ -3258,7 +3855,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H64" s="6">
         <v>9</v>
@@ -3267,18 +3864,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:9">
       <c r="A65" s="6">
         <v>100061</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>203</v>
+        <v>239</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>204</v>
+        <v>240</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>205</v>
+        <v>241</v>
       </c>
       <c r="E65" s="6">
         <v>2</v>
@@ -3287,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H65" s="6">
         <v>10</v>
@@ -3296,18 +3893,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:9">
       <c r="A66" s="6">
         <v>100062</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>206</v>
+        <v>242</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>207</v>
+        <v>243</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>208</v>
+        <v>244</v>
       </c>
       <c r="E66" s="6">
         <v>2</v>
@@ -3316,7 +3913,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H66" s="6">
         <v>11</v>
@@ -3325,18 +3922,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:9">
       <c r="A67" s="6">
         <v>100063</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="E67" s="6">
         <v>2</v>
@@ -3345,7 +3942,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H67" s="6">
         <v>12</v>
@@ -3354,18 +3951,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:9">
       <c r="A68" s="6">
         <v>100064</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>212</v>
+        <v>248</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>213</v>
+        <v>249</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="E68" s="6">
         <v>2</v>
@@ -3374,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H68" s="6">
         <v>13</v>
@@ -3383,18 +3980,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9">
       <c r="A69" s="6">
         <v>100065</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>215</v>
+        <v>251</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>216</v>
+        <v>252</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
       <c r="E69" s="6">
         <v>2</v>
@@ -3403,7 +4000,7 @@
         <v>1</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H69" s="6">
         <v>14</v>
@@ -3412,18 +4009,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:9">
       <c r="A70" s="6">
         <v>100066</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>218</v>
+        <v>254</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>220</v>
+        <v>256</v>
       </c>
       <c r="E70" s="6">
         <v>2</v>
@@ -3432,7 +4029,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H70" s="6">
         <v>17</v>
@@ -3441,18 +4038,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:9">
       <c r="A71" s="6">
         <v>100067</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>221</v>
+        <v>257</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>222</v>
+        <v>258</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="E71" s="6">
         <v>2</v>
@@ -3461,7 +4058,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H71" s="6">
         <v>18</v>
@@ -3470,18 +4067,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:9">
       <c r="A72" s="6">
         <v>100068</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>224</v>
+        <v>260</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>226</v>
+        <v>262</v>
       </c>
       <c r="E72" s="6">
         <v>2</v>
@@ -3490,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H72" s="6">
         <v>19</v>
@@ -3499,18 +4096,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:9">
       <c r="A73" s="6">
         <v>100069</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>227</v>
+        <v>263</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="E73" s="6">
         <v>2</v>
@@ -3519,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H73" s="6">
         <v>21</v>
@@ -3528,18 +4125,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:9">
       <c r="A74" s="6">
         <v>100070</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>231</v>
+        <v>267</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>232</v>
+        <v>268</v>
       </c>
       <c r="E74" s="6">
         <v>2</v>
@@ -3548,7 +4145,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
       <c r="H74" s="6">
         <v>20</v>
@@ -3557,18 +4154,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:9">
       <c r="A75" s="6">
         <v>100071</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>233</v>
+        <v>269</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>234</v>
+        <v>270</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>235</v>
+        <v>271</v>
       </c>
       <c r="E75" s="6">
         <v>2</v>
@@ -3577,7 +4174,7 @@
         <v>1</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H75" s="6">
         <v>15</v>
@@ -3586,18 +4183,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:9">
       <c r="A76" s="6">
         <v>100072</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>236</v>
+        <v>273</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>238</v>
+        <v>275</v>
       </c>
       <c r="E76" s="6">
         <v>2</v>
@@ -3606,7 +4203,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>242</v>
+        <v>276</v>
       </c>
       <c r="H76" s="6">
         <v>2</v>
@@ -3615,18 +4212,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:9">
       <c r="A77" s="6">
         <v>100073</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>239</v>
+        <v>277</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>240</v>
+        <v>278</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="E77" s="6">
         <v>2</v>
@@ -3635,7 +4232,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="H77" s="6">
         <v>25</v>
@@ -3645,8 +4242,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: daily level up
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Task_任务.xlsx
+++ b/nevergiveup/Excel/Task_任务.xlsx
@@ -2105,9 +2105,9 @@
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="H82" sqref="H82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -4177,7 +4177,7 @@
         <v>272</v>
       </c>
       <c r="H75" s="6">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I75" s="6">
         <v>1</v>

</xml_diff>